<commit_message>
Begins introducing our own cell types by the 'STRING' type.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3D458C-7829-4F32-9E10-3136E86C0ED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0010008F-4366-4743-9246-434534868158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="6180" windowWidth="15660" windowHeight="11145" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="28785" yWindow="5145" windowWidth="15750" windowHeight="12600" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CellWorksheet" sheetId="27" r:id="rId1"/>
@@ -455,39 +455,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="3.140625" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="D1" t="str">
+        <f>_xlfn.CONCAT(C1,C1)</f>
+        <v>StringString</v>
+      </c>
+      <c r="E1">
         <v>1</v>
       </c>
-      <c r="C1">
+      <c r="F1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D1" s="3">
+      <c r="G1" s="3">
         <v>39757</v>
       </c>
-      <c r="E1" s="4">
+      <c r="H1" s="4">
         <v>1</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="5"/>
-      <c r="H1" t="str">
-        <f>_xlfn.CONCAT(A1,A1)</f>
-        <v>StringString</v>
-      </c>
       <c r="I1">
-        <f>B1+B1</f>
+        <f>E1+E1</f>
         <v>2</v>
       </c>
       <c r="J1">
-        <f>C1+C1</f>
+        <f>F1+F1</f>
         <v>2.2000000000000002</v>
       </c>
       <c r="K1" t="s">

</xml_diff>

<commit_message>
Introduces the 'INTEGER' 'Cell' type.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0010008F-4366-4743-9246-434534868158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2A5B8A-F9A3-4F1F-A861-2DCD01279CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28785" yWindow="5145" windowWidth="15750" windowHeight="12600" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>Andrei Diego Cardoso</author>
   </authors>
   <commentList>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
+    <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -128,13 +128,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -449,9 +451,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA818CB8-6D84-47CC-9931-F9A2D8F9098F}">
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -459,19 +463,20 @@
     <col min="2" max="2" width="3.140625" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.85546875" customWidth="1"/>
+    <col min="12" max="12" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="5"/>
+      <c r="B1" s="4"/>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -483,29 +488,43 @@
         <v>1</v>
       </c>
       <c r="F1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G1" s="3">
-        <v>39757</v>
-      </c>
-      <c r="H1" s="4">
-        <v>1</v>
-      </c>
-      <c r="I1">
         <f>E1+E1</f>
         <v>2</v>
       </c>
+      <c r="G1" s="5">
+        <v>1</v>
+      </c>
+      <c r="H1" s="6" t="str">
+        <f>_xlfn.CONCAT(G1,G1)</f>
+        <v>11</v>
+      </c>
+      <c r="I1">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="J1">
-        <f>F1+F1</f>
+        <f>I1+I1</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L1" s="6" t="str">
+        <f>_xlfn.CONCAT(1,",1")</f>
+        <v>1,1</v>
+      </c>
+      <c r="M1" s="3">
+        <v>39757</v>
+      </c>
+      <c r="N1" s="7">
+        <v>1</v>
+      </c>
+      <c r="O1" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Introduces the 'DOUBLE' 'Cell' type.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2A5B8A-F9A3-4F1F-A861-2DCD01279CBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEF058E-0024-47AD-BB7A-1E03C9AFCC9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28785" yWindow="5145" windowWidth="15750" windowHeight="12600" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="-16965" yWindow="2610" windowWidth="15750" windowHeight="12600" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CellWorksheet" sheetId="27" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Andrei Diego Cardoso</author>
   </authors>
   <commentList>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
       <text>
         <r>
           <rPr>
@@ -58,12 +58,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>String</t>
   </si>
   <si>
     <t>Automatic</t>
+  </si>
+  <si>
+    <t>1.1</t>
+  </si>
+  <si>
+    <t>1,1</t>
   </si>
 </sst>
 </file>
@@ -128,15 +134,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,30 +456,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA818CB8-6D84-47CC-9931-F9A2D8F9098F}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="3.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" customWidth="1"/>
     <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.85546875" customWidth="1"/>
+    <col min="9" max="11" width="4" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" t="s">
@@ -491,11 +497,11 @@
         <f>E1+E1</f>
         <v>2</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="6">
         <v>1</v>
       </c>
-      <c r="H1" s="6" t="str">
-        <f>_xlfn.CONCAT(G1,G1)</f>
+      <c r="H1" t="str">
+        <f>_xlfn.CONCAT(1,1)</f>
         <v>11</v>
       </c>
       <c r="I1">
@@ -505,32 +511,42 @@
         <f>I1+I1</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="K1" s="5">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="L1" s="6" t="str">
-        <f>_xlfn.CONCAT(1,",1")</f>
+      <c r="K1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="str">
+        <f>_xlfn.CONCAT("1.",1)</f>
+        <v>1.1</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="str">
+        <f>_xlfn.CONCAT("1,",1)</f>
         <v>1,1</v>
       </c>
-      <c r="M1" s="3">
+      <c r="O1" s="3">
         <v>39757</v>
       </c>
-      <c r="N1" s="7">
+      <c r="P1" s="5">
         <v>1</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="M1" numberStoredAsText="1"/>
+  </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Introduces the 'DATE' 'Cell' type.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3359D3A3-893C-4003-AED0-C1CDB774753D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDB814-F015-4B25-9523-E983A70E7AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15285" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CellWorksheet" sheetId="27" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Andrei Diego Cardoso</author>
   </authors>
   <commentList>
-    <comment ref="AA1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
+    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>String</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>1.1</t>
+  </si>
+  <si>
+    <t>05/11/2008</t>
   </si>
   <si>
     <t>R$ 1,00</t>
@@ -82,14 +85,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="5" formatCode="&quot;R$&quot;\ #,##0;\-&quot;R$&quot;\ #,##0"/>
     <numFmt numFmtId="6" formatCode="&quot;R$&quot;\ #,##0;[Red]\-&quot;R$&quot;\ #,##0"/>
     <numFmt numFmtId="7" formatCode="&quot;R$&quot;\ #,##0.00;\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="42" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="&quot;R$&quot;\ #,##0.00;[Red]&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -146,21 +148,40 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="5" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,9 +496,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA818CB8-6D84-47CC-9931-F9A2D8F9098F}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:BE1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AE1" sqref="AE1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -488,20 +511,41 @@
     <col min="5" max="7" width="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="6" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="25" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="25" width="7.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="29" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" t="s">
@@ -518,7 +562,7 @@
         <f>E1+E1</f>
         <v>2</v>
       </c>
-      <c r="G1" s="13">
+      <c r="G1" s="27">
         <v>1</v>
       </c>
       <c r="H1" t="str">
@@ -532,15 +576,15 @@
         <f>I1+I1</f>
         <v>2.2000000000000002</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="27" t="s">
         <v>2</v>
       </c>
       <c r="L1" t="str">
         <f>_xlfn.CONCAT("1.",1)</f>
         <v>1.1</v>
       </c>
-      <c r="M1" s="13" t="s">
-        <v>4</v>
+      <c r="M1" s="27" t="s">
+        <v>5</v>
       </c>
       <c r="N1" t="str">
         <f>_xlfn.CONCAT("1,",1)</f>
@@ -564,36 +608,80 @@
       <c r="T1" s="11">
         <v>1</v>
       </c>
-      <c r="U1" s="5">
+      <c r="U1" s="11">
         <f>T1+T1</f>
         <v>2</v>
       </c>
-      <c r="V1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="12" t="str">
+      <c r="V1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="W1" s="26" t="str">
         <f>_xlfn.CONCAT("R$ ","1.00")</f>
         <v>R$ 1.00</v>
       </c>
-      <c r="X1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y1" s="12" t="str">
+      <c r="X1" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y1" s="26" t="str">
         <f>_xlfn.CONCAT("R$ ","1,00")</f>
         <v>R$ 1,00</v>
       </c>
       <c r="Z1" s="3">
         <v>39757</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="28">
+        <v>39757</v>
+      </c>
+      <c r="AB1" s="29">
+        <v>39757</v>
+      </c>
+      <c r="AC1" s="30">
+        <v>39757</v>
+      </c>
+      <c r="AD1" s="31">
+        <v>39757</v>
+      </c>
+      <c r="AE1" s="3">
+        <f>AD1+1</f>
+        <v>39758</v>
+      </c>
+      <c r="AF1" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="AG1" s="3" t="str">
+        <f>_xlfn.CONCAT("05","/",11,"/",2008)</f>
+        <v>05/11/2008</v>
+      </c>
+      <c r="AH1" t="s">
         <v>0</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AC1" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="12"/>
+      <c r="AQ1" s="13"/>
+      <c r="AR1" s="14"/>
+      <c r="AS1" s="15"/>
+      <c r="AT1" s="16"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="18"/>
+      <c r="AW1" s="19"/>
+      <c r="AX1" s="20"/>
+      <c r="AY1" s="21"/>
+      <c r="AZ1" s="22"/>
+      <c r="BA1" s="23"/>
+      <c r="BB1" s="24"/>
+      <c r="BC1" s="25"/>
+      <c r="BD1" s="32"/>
+      <c r="BE1" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prevents an invalid date cell from being created from a negative value.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDB814-F015-4B25-9523-E983A70E7AC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EC31FD-70FC-490C-B481-601865FF5D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="12600" windowWidth="15750" windowHeight="12600" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15285" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CellWorksheet" sheetId="27" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Andrei Diego Cardoso</author>
   </authors>
   <commentList>
-    <comment ref="AH1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
+    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
       <text>
         <r>
           <rPr>
@@ -496,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA818CB8-6D84-47CC-9931-F9A2D8F9098F}">
-  <dimension ref="A1:BE1"/>
+  <dimension ref="A1:BF1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,7 +524,8 @@
     <col min="30" max="30" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.140625" customWidth="1"/>
+    <col min="35" max="35" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="33.85546875" bestFit="1" customWidth="1"/>
@@ -545,7 +546,7 @@
     <col min="56" max="56" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" t="s">
@@ -652,36 +653,39 @@
         <f>_xlfn.CONCAT("05","/",11,"/",2008)</f>
         <v>05/11/2008</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="3">
+        <v>-39757</v>
+      </c>
+      <c r="AI1" t="s">
         <v>0</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK1" s="3"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="30"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="14"/>
-      <c r="AS1" s="15"/>
-      <c r="AT1" s="16"/>
-      <c r="AU1" s="17"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="19"/>
-      <c r="AX1" s="20"/>
-      <c r="AY1" s="21"/>
-      <c r="AZ1" s="22"/>
-      <c r="BA1" s="23"/>
-      <c r="BB1" s="24"/>
-      <c r="BC1" s="25"/>
-      <c r="BD1" s="32"/>
+      <c r="AK1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="12"/>
+      <c r="AR1" s="13"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="16"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="18"/>
+      <c r="AX1" s="19"/>
+      <c r="AY1" s="20"/>
+      <c r="AZ1" s="21"/>
+      <c r="BA1" s="22"/>
+      <c r="BB1" s="23"/>
+      <c r="BC1" s="24"/>
+      <c r="BD1" s="25"/>
       <c r="BE1" s="32"/>
+      <c r="BF1" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prevents an invalid date cell from being created from a value that resembles a date but has unexpected characters (other than numbers and the '/' symbol) in it.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8EC31FD-70FC-490C-B481-601865FF5D6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8FB73D-9A4B-436F-9B85-EC9B6CCCC2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15285" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="30" yWindow="30" windowWidth="14400" windowHeight="15285" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CellWorksheet" sheetId="27" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Andrei Diego Cardoso</author>
   </authors>
   <commentList>
-    <comment ref="AI1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
+    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>String</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>R$ 1.00</t>
+  </si>
+  <si>
+    <t>O5/11/2008</t>
   </si>
 </sst>
 </file>
@@ -496,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA818CB8-6D84-47CC-9931-F9A2D8F9098F}">
-  <dimension ref="A1:BF1"/>
+  <dimension ref="A1:BG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AI1" sqref="AI1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,28 +528,26 @@
     <col min="31" max="31" width="10.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8.140625" customWidth="1"/>
-    <col min="35" max="35" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" t="s">
@@ -656,36 +657,39 @@
       <c r="AH1" s="3">
         <v>-39757</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>0</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AK1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL1" s="3"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="30"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="14"/>
-      <c r="AT1" s="15"/>
-      <c r="AU1" s="16"/>
-      <c r="AV1" s="17"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="19"/>
-      <c r="AY1" s="20"/>
-      <c r="AZ1" s="21"/>
-      <c r="BA1" s="22"/>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="24"/>
-      <c r="BD1" s="25"/>
-      <c r="BE1" s="32"/>
+      <c r="AL1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="28"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="12"/>
+      <c r="AS1" s="13"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="16"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="18"/>
+      <c r="AY1" s="19"/>
+      <c r="AZ1" s="20"/>
+      <c r="BA1" s="21"/>
+      <c r="BB1" s="22"/>
+      <c r="BC1" s="23"/>
+      <c r="BD1" s="24"/>
+      <c r="BE1" s="25"/>
       <c r="BF1" s="32"/>
+      <c r="BG1" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Prevents an invalid date cell from being created from an invalid date value.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8FB73D-9A4B-436F-9B85-EC9B6CCCC2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A2391-1394-4F21-B0F7-DF8191E032DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="30" windowWidth="14400" windowHeight="15285" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15285" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CellWorksheet" sheetId="27" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Andrei Diego Cardoso</author>
   </authors>
   <commentList>
-    <comment ref="AJ1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
+    <comment ref="AK1" authorId="0" shapeId="0" xr:uid="{5393BACB-465E-47B0-B46A-0A95784F4D8C}">
       <text>
         <r>
           <rPr>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>String</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>O5/11/2008</t>
+  </si>
+  <si>
+    <t>05/13/2008</t>
   </si>
 </sst>
 </file>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA818CB8-6D84-47CC-9931-F9A2D8F9098F}">
-  <dimension ref="A1:BG1"/>
+  <dimension ref="A1:BH1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AI1" sqref="AI1"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,9 +532,9 @@
     <col min="32" max="33" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="8.140625" customWidth="1"/>
     <col min="35" max="35" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="33.85546875" bestFit="1" customWidth="1"/>
@@ -547,7 +550,7 @@
     <col min="55" max="55" width="33.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="4"/>
       <c r="C1" t="s">
@@ -660,36 +663,39 @@
       <c r="AI1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK1" t="s">
         <v>0</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AL1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM1" s="3"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="30"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="14"/>
-      <c r="AU1" s="15"/>
-      <c r="AV1" s="16"/>
-      <c r="AW1" s="17"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="19"/>
-      <c r="AZ1" s="20"/>
-      <c r="BA1" s="21"/>
-      <c r="BB1" s="22"/>
-      <c r="BC1" s="23"/>
-      <c r="BD1" s="24"/>
-      <c r="BE1" s="25"/>
-      <c r="BF1" s="32"/>
+      <c r="AM1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN1" s="3"/>
+      <c r="AO1" s="28"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="12"/>
+      <c r="AT1" s="13"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="15"/>
+      <c r="AW1" s="16"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="18"/>
+      <c r="AZ1" s="19"/>
+      <c r="BA1" s="20"/>
+      <c r="BB1" s="21"/>
+      <c r="BC1" s="22"/>
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="24"/>
+      <c r="BF1" s="25"/>
       <c r="BG1" s="32"/>
+      <c r="BH1" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Introduces the capability of ingesting cells with error as 'STRING' 'Cell's.
</commit_message>
<xml_diff>
--- a/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
+++ b/code/stocks/src/test/resources/com/andreidiego/mpfi/stocks/adapter/spreadsheets/excel/poi/Cell.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\Projects\Personal\MPFi\code\stocks\src\test\resources\com\andreidiego\mpfi\stocks\adapter\spreadsheets\excel\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48A2391-1394-4F21-B0F7-DF8191E032DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C183A18C-C7EE-4EE3-AC23-91F01B3C983C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15285" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
+    <workbookView xWindow="3120" yWindow="915" windowWidth="14400" windowHeight="15285" xr2:uid="{2B1CA52D-E10F-49D8-8A0A-7B3A987640D9}"/>
   </bookViews>
   <sheets>
     <sheet name="CellWorksheet" sheetId="27" r:id="rId1"/>
@@ -55,6 +55,28 @@
     </comment>
   </commentList>
 </comments>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,7 +527,7 @@
   <dimension ref="A1:BH1"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AM1" sqref="AM1"/>
+      <selection activeCell="AN1" sqref="AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +557,7 @@
     <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="37" max="38" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="43" max="43" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -675,7 +697,10 @@
       <c r="AM1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AN1" s="3"/>
+      <c r="AN1" s="3" t="e" cm="1">
+        <f t="array" ref="AN1">l+1</f>
+        <v>#NAME?</v>
+      </c>
       <c r="AO1" s="28"/>
       <c r="AP1" s="29"/>
       <c r="AQ1" s="30"/>

</xml_diff>